<commit_message>
Actualizacion de documentos versiones finales
</commit_message>
<xml_diff>
--- a/Documentacion/PREGAME/1. ELICITACION/1.3 Historias Usuario/G3_Ceron_Chicaiza_Llorente_PT1_Matriz HU002.xlsx
+++ b/Documentacion/PREGAME/1. ELICITACION/1.3 Historias Usuario/G3_Ceron_Chicaiza_Llorente_PT1_Matriz HU002.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. ESPE\6. SEMESTRE\02_ANALISIS Y DISENO DE SOFTWARE\PROYECTO\3712_G3_CeronChicaizaLlorente_GJenga\Documentacion\PREGAME\1. ELICITACION\1.3 Historias Usuario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B3C7D8-7DCF-47DD-A1F5-2039A0EE9A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D4CC8E-39C3-452B-8BBC-C5B8C2E54872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formato descripción HU" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="78">
   <si>
     <t>Matriz de Marco de Trabajo de HU</t>
   </si>
@@ -101,10 +101,6 @@
     <t>Usuario</t>
   </si>
   <si>
-    <t>1. Agregar la cantidad del producto a comprar.
-2. Dar clic en el boton "Añadir al carrito"</t>
-  </si>
-  <si>
     <t>Maria Belen Ceron</t>
   </si>
   <si>
@@ -155,10 +151,6 @@
   </si>
   <si>
     <t>Pagar productos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Dar clic en el visualizar pago.
-2. Click en "Aceptar" (cuadro de informacion que muestra el total en dolares). </t>
   </si>
   <si>
     <t>Elian Llorente</t>
@@ -247,14 +239,53 @@
   <si>
     <t>PRUEBA</t>
   </si>
+  <si>
+    <t>1. Agregar la cantidad del producto a comprar.
+2. Dar clic en el boton "Agregar al carrito"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Dar clic en el boton "Ver Carrito".
+2. Click en "Siguiente" (cuadro de informacion que muestra el total en dolares). </t>
+  </si>
+  <si>
+    <t>El aplicativo debera permitir que el usuario ingrese sus datos personales(Nombre, Telefono, Direccion)</t>
+  </si>
+  <si>
+    <t>Identificar los productos que han sido pedidos por determinado usuario</t>
+  </si>
+  <si>
+    <t>1. Ingresar los datos personales del usuario en el formulario (Nombre, Telefono y Direccion)
+2. Dar click en "Siguiente"</t>
+  </si>
+  <si>
+    <t>Verificar que el usuario nuevo se haya registrado correctamente en la base de datos y usar pruebas unitarias</t>
+  </si>
+  <si>
+    <t>Registrar el pedido</t>
+  </si>
+  <si>
+    <t>El aplicativo debera permitir que el usuario realice su pedido</t>
+  </si>
+  <si>
+    <t>Registrar de manera automatica un determinado pedido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Dar clic en "Ordenar"
+</t>
+  </si>
+  <si>
+    <t>Verificar que el pedido, detalle del pedido se hayan registrado en la base de datos correctamente y usar pruebas unitarias</t>
+  </si>
+  <si>
+    <t>Registrar al cliente</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="165" formatCode="d/m"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -759,7 +790,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -796,9 +827,6 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -821,9 +849,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -876,34 +901,41 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -912,13 +944,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1257,8 +1282,8 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1310,22 +1335,22 @@
     </row>
     <row r="3" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
+      <c r="N3" s="45"/>
+      <c r="O3" s="45"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
@@ -1418,10 +1443,10 @@
         <v>19</v>
       </c>
       <c r="G6" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>20</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="I6" s="12">
         <v>8</v>
@@ -1430,40 +1455,40 @@
         <v>44405</v>
       </c>
       <c r="K6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="M6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="M6" s="14" t="s">
+      <c r="N6" s="14"/>
+      <c r="O6" s="15" t="s">
         <v>24</v>
-      </c>
-      <c r="N6" s="15"/>
-      <c r="O6" s="16" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="E7" s="9" t="s">
         <v>28</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>29</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>19</v>
       </c>
       <c r="G7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>30</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>31</v>
       </c>
       <c r="I7" s="12">
         <v>6</v>
@@ -1472,112 +1497,160 @@
         <v>44406</v>
       </c>
       <c r="K7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="17" t="s">
-        <v>23</v>
-      </c>
       <c r="M7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" s="9"/>
+      <c r="O7" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="N7" s="9"/>
-      <c r="O7" s="18" t="s">
+    </row>
+    <row r="8" spans="1:26" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="8" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="D8" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="E8" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="F8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="H8" s="21" t="s">
+      <c r="I8" s="16">
+        <v>6</v>
+      </c>
+      <c r="J8" s="21">
+        <v>44426</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="10" t="s">
         <v>39</v>
-      </c>
-      <c r="I8" s="17">
-        <v>6</v>
-      </c>
-      <c r="J8" s="22">
-        <v>44426</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L8" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>41</v>
       </c>
       <c r="N8" s="9"/>
       <c r="O8" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="19"/>
-      <c r="S8" s="19"/>
-      <c r="T8" s="19"/>
-      <c r="U8" s="19"/>
-      <c r="V8" s="19"/>
-      <c r="W8" s="19"/>
-      <c r="X8" s="19"/>
-      <c r="Y8" s="19"/>
-      <c r="Z8" s="19"/>
+        <v>40</v>
+      </c>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="18"/>
+      <c r="T8" s="18"/>
+      <c r="U8" s="18"/>
+      <c r="V8" s="18"/>
+      <c r="W8" s="18"/>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="18"/>
+      <c r="Z8" s="18"/>
     </row>
     <row r="9" spans="1:26" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="9"/>
+        <v>41</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="12">
+        <v>8</v>
+      </c>
+      <c r="J9" s="13">
+        <v>44443</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>71</v>
+      </c>
       <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
+      <c r="O9" s="9" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="9"/>
+        <v>42</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="12">
+        <v>8</v>
+      </c>
+      <c r="J10" s="13">
+        <v>44445</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>76</v>
+      </c>
       <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
+      <c r="O10" s="9" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -1595,7 +1668,7 @@
     </row>
     <row r="12" spans="1:26" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -1613,7 +1686,7 @@
     </row>
     <row r="13" spans="1:26" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -1631,7 +1704,7 @@
     </row>
     <row r="14" spans="1:26" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -1649,7 +1722,7 @@
     </row>
     <row r="15" spans="1:26" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -1667,7 +1740,7 @@
     </row>
     <row r="16" spans="1:26" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
@@ -1685,7 +1758,7 @@
     </row>
     <row r="17" spans="2:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -1703,7 +1776,7 @@
     </row>
     <row r="18" spans="2:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
@@ -1721,7 +1794,7 @@
     </row>
     <row r="19" spans="2:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -1739,7 +1812,7 @@
     </row>
     <row r="20" spans="2:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -1765,7 +1838,7 @@
       <c r="H21" s="4"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
-      <c r="K21" s="24"/>
+      <c r="K21" s="22"/>
       <c r="L21" s="3"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
@@ -1791,13 +1864,13 @@
     <row r="25" spans="2:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
-      <c r="K25" s="25"/>
+      <c r="K25" s="23"/>
       <c r="L25" s="3"/>
     </row>
     <row r="26" spans="2:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
-      <c r="K26" s="25"/>
+      <c r="K26" s="23"/>
       <c r="L26" s="3"/>
     </row>
     <row r="27" spans="2:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1822,10 +1895,10 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M30" s="5"/>
     </row>
@@ -1833,10 +1906,10 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M31" s="5"/>
     </row>
@@ -1844,10 +1917,10 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M32" s="5"/>
     </row>
@@ -1856,7 +1929,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="2"/>
       <c r="L33" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="M33" s="5"/>
     </row>
@@ -7659,13 +7732,13 @@
     <row r="1000" spans="9:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1000" s="3"/>
       <c r="J1000" s="3"/>
-      <c r="K1000" s="24"/>
+      <c r="K1000" s="22"/>
       <c r="L1000" s="3"/>
     </row>
     <row r="1001" spans="9:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1001" s="3"/>
       <c r="J1001" s="3"/>
-      <c r="K1001" s="24"/>
+      <c r="K1001" s="22"/>
       <c r="L1001" s="3"/>
     </row>
   </sheetData>
@@ -7693,7 +7766,9 @@
   </sheetPr>
   <dimension ref="A2:Z1020"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="S23" sqref="S23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7707,52 +7782,52 @@
     <row r="2" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:26" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="71" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="72"/>
-      <c r="M6" s="72"/>
-      <c r="N6" s="72"/>
-      <c r="O6" s="72"/>
-      <c r="P6" s="58"/>
+      <c r="B6" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="60"/>
+      <c r="O6" s="60"/>
+      <c r="P6" s="61"/>
     </row>
     <row r="7" spans="1:26" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27"/>
-      <c r="O7" s="27"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
@@ -7766,90 +7841,90 @@
       <c r="Z7" s="4"/>
     </row>
     <row r="8" spans="1:26" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="28"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="32"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="30"/>
       <c r="Q8" s="4"/>
     </row>
     <row r="9" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="33"/>
-      <c r="C9" s="34" t="s">
+      <c r="B9" s="31"/>
+      <c r="C9" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="57" t="s">
-        <v>60</v>
-      </c>
-      <c r="F9" s="58"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="57" t="s">
+      <c r="D9" s="33"/>
+      <c r="E9" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="61"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="58"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="37"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="35"/>
       <c r="Q9" s="4"/>
     </row>
     <row r="10" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="33"/>
-      <c r="C10" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="39"/>
-      <c r="E10" s="59" t="str">
+      <c r="B10" s="31"/>
+      <c r="C10" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="37"/>
+      <c r="E10" s="63" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O20,5,0)</f>
         <v>Usuario</v>
       </c>
-      <c r="F10" s="58"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="59" t="str">
+      <c r="F10" s="61"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="63" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O20,11,0)</f>
         <v>Terminado</v>
       </c>
-      <c r="I10" s="58"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="36"/>
-      <c r="N10" s="36"/>
-      <c r="O10" s="36"/>
-      <c r="P10" s="37"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="35"/>
       <c r="Q10" s="4"/>
     </row>
     <row r="11" spans="1:26" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="36"/>
-      <c r="N11" s="42"/>
-      <c r="O11" s="42"/>
-      <c r="P11" s="37"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="40"/>
+      <c r="O11" s="40"/>
+      <c r="P11" s="35"/>
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
@@ -7863,27 +7938,27 @@
     </row>
     <row r="12" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="57" t="s">
+      <c r="B12" s="31"/>
+      <c r="C12" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="37"/>
+      <c r="E12" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="58"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="57" t="s">
-        <v>62</v>
-      </c>
-      <c r="I12" s="58"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="42"/>
-      <c r="O12" s="42"/>
-      <c r="P12" s="37"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="62" t="s">
+        <v>60</v>
+      </c>
+      <c r="I12" s="61"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="40"/>
+      <c r="O12" s="40"/>
+      <c r="P12" s="35"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
@@ -7897,30 +7972,30 @@
     </row>
     <row r="13" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="38">
+      <c r="B13" s="31"/>
+      <c r="C13" s="36">
         <f>VLOOKUP('Historia de Usuario'!C10,'Formato descripción HU'!B6:O20,8,0)</f>
         <v>8</v>
       </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="59" t="str">
+      <c r="D13" s="37"/>
+      <c r="E13" s="63" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O20,10,0)</f>
         <v>Alta</v>
       </c>
-      <c r="F13" s="58"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="59" t="str">
+      <c r="F13" s="61"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="63" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O20,7,0)</f>
         <v>Maria Belen Ceron</v>
       </c>
-      <c r="I13" s="58"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="36"/>
-      <c r="N13" s="42"/>
-      <c r="O13" s="42"/>
-      <c r="P13" s="37"/>
+      <c r="I13" s="61"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="35"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
@@ -7934,21 +8009,21 @@
     </row>
     <row r="14" spans="1:26" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="36"/>
-      <c r="O14" s="36"/>
-      <c r="P14" s="37"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="35"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
@@ -7962,37 +8037,37 @@
     </row>
     <row r="15" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="61" t="s">
+      <c r="B15" s="31"/>
+      <c r="C15" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="64" t="str">
+        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O20,3,0)</f>
+        <v>Registrar el pedido</v>
+      </c>
+      <c r="E15" s="50"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="H15" s="64" t="str">
+        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O20,4,0)</f>
+        <v>Registrar de manera automatica un determinado pedido</v>
+      </c>
+      <c r="I15" s="57"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="60" t="str">
-        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O20,3,0)</f>
-        <v>Agregar productos al carrito de compras</v>
-      </c>
-      <c r="E15" s="49"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="61" t="s">
-        <v>64</v>
-      </c>
-      <c r="H15" s="60" t="str">
-        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O20,4,0)</f>
-        <v>Realizar compras mediante el aplicativo</v>
-      </c>
-      <c r="I15" s="55"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="61" t="s">
-        <v>65</v>
-      </c>
-      <c r="M15" s="54" t="str">
+      <c r="M15" s="56" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O20,6,0)</f>
-        <v>1. Agregar la cantidad del producto a comprar.
-2. Dar clic en el boton "Añadir al carrito"</v>
-      </c>
-      <c r="N15" s="55"/>
-      <c r="O15" s="49"/>
-      <c r="P15" s="37"/>
+        <v xml:space="preserve">1. Dar clic en "Ordenar"
+</v>
+      </c>
+      <c r="N15" s="57"/>
+      <c r="O15" s="50"/>
+      <c r="P15" s="35"/>
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
@@ -8006,21 +8081,21 @@
     </row>
     <row r="16" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="51"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="62"/>
-      <c r="M16" s="50"/>
-      <c r="N16" s="47"/>
-      <c r="O16" s="51"/>
-      <c r="P16" s="37"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="55"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="54"/>
+      <c r="N16" s="45"/>
+      <c r="O16" s="55"/>
+      <c r="P16" s="35"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
@@ -8034,21 +8109,21 @@
     </row>
     <row r="17" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="56"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="36"/>
-      <c r="L17" s="63"/>
-      <c r="M17" s="52"/>
-      <c r="N17" s="56"/>
-      <c r="O17" s="53"/>
-      <c r="P17" s="37"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="51"/>
+      <c r="N17" s="58"/>
+      <c r="O17" s="52"/>
+      <c r="P17" s="35"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
@@ -8062,21 +8137,21 @@
     </row>
     <row r="18" spans="1:26" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="36"/>
-      <c r="K18" s="36"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="36"/>
-      <c r="N18" s="36"/>
-      <c r="O18" s="36"/>
-      <c r="P18" s="37"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="34"/>
+      <c r="O18" s="34"/>
+      <c r="P18" s="35"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
@@ -8089,91 +8164,91 @@
       <c r="Z18" s="4"/>
     </row>
     <row r="19" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="33"/>
-      <c r="C19" s="70" t="s">
-        <v>66</v>
-      </c>
-      <c r="D19" s="49"/>
-      <c r="E19" s="64" t="str">
+      <c r="B19" s="31"/>
+      <c r="C19" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="50"/>
+      <c r="E19" s="65" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O20,14,0)</f>
-        <v>Agregar productos al carrito de compra</v>
-      </c>
-      <c r="F19" s="65"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="65"/>
-      <c r="I19" s="65"/>
-      <c r="J19" s="65"/>
-      <c r="K19" s="65"/>
-      <c r="L19" s="65"/>
-      <c r="M19" s="65"/>
-      <c r="N19" s="65"/>
-      <c r="O19" s="66"/>
-      <c r="P19" s="37"/>
+        <v>Registrar el pedido</v>
+      </c>
+      <c r="F19" s="66"/>
+      <c r="G19" s="66"/>
+      <c r="H19" s="66"/>
+      <c r="I19" s="66"/>
+      <c r="J19" s="66"/>
+      <c r="K19" s="66"/>
+      <c r="L19" s="66"/>
+      <c r="M19" s="66"/>
+      <c r="N19" s="66"/>
+      <c r="O19" s="67"/>
+      <c r="P19" s="35"/>
       <c r="Q19" s="4"/>
     </row>
     <row r="20" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="33"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="67"/>
-      <c r="F20" s="68"/>
-      <c r="G20" s="68"/>
-      <c r="H20" s="68"/>
-      <c r="I20" s="68"/>
-      <c r="J20" s="68"/>
-      <c r="K20" s="68"/>
-      <c r="L20" s="68"/>
-      <c r="M20" s="68"/>
-      <c r="N20" s="68"/>
-      <c r="O20" s="69"/>
-      <c r="P20" s="37"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="69"/>
+      <c r="G20" s="69"/>
+      <c r="H20" s="69"/>
+      <c r="I20" s="69"/>
+      <c r="J20" s="69"/>
+      <c r="K20" s="69"/>
+      <c r="L20" s="69"/>
+      <c r="M20" s="69"/>
+      <c r="N20" s="69"/>
+      <c r="O20" s="70"/>
+      <c r="P20" s="35"/>
       <c r="Q20" s="4"/>
     </row>
     <row r="21" spans="1:26" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="33"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="36"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="36"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="36"/>
-      <c r="N21" s="36"/>
-      <c r="O21" s="36"/>
-      <c r="P21" s="37"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="34"/>
+      <c r="P21" s="35"/>
       <c r="Q21" s="4"/>
     </row>
     <row r="22" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="49"/>
-      <c r="E22" s="54" t="str">
+      <c r="B22" s="31"/>
+      <c r="C22" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="50"/>
+      <c r="E22" s="56" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O20,12,0)</f>
-        <v>Verificar que en el carrito de compras se haya añadido de manera correcta el producto seleccionado (Producto, cantidad,precio unitario, precio total) y ademas el uso de pruebas unitarias</v>
-      </c>
-      <c r="F22" s="55"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="48" t="s">
+        <v>Verificar que el pedido, detalle del pedido se hayan registrado en la base de datos correctamente y usar pruebas unitarias</v>
+      </c>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="K22" s="49"/>
-      <c r="L22" s="54">
+      <c r="K22" s="50"/>
+      <c r="L22" s="56">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O20,13,0)</f>
         <v>0</v>
       </c>
-      <c r="M22" s="55"/>
-      <c r="N22" s="55"/>
-      <c r="O22" s="49"/>
-      <c r="P22" s="37"/>
+      <c r="M22" s="57"/>
+      <c r="N22" s="57"/>
+      <c r="O22" s="50"/>
+      <c r="P22" s="35"/>
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
@@ -8187,21 +8262,21 @@
     </row>
     <row r="23" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="51"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="50"/>
-      <c r="K23" s="51"/>
-      <c r="L23" s="50"/>
-      <c r="M23" s="47"/>
-      <c r="N23" s="47"/>
-      <c r="O23" s="51"/>
-      <c r="P23" s="37"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="55"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="55"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="45"/>
+      <c r="N23" s="45"/>
+      <c r="O23" s="55"/>
+      <c r="P23" s="35"/>
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
@@ -8215,21 +8290,21 @@
     </row>
     <row r="24" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="56"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="53"/>
-      <c r="L24" s="52"/>
-      <c r="M24" s="56"/>
-      <c r="N24" s="56"/>
-      <c r="O24" s="53"/>
-      <c r="P24" s="37"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="51"/>
+      <c r="M24" s="58"/>
+      <c r="N24" s="58"/>
+      <c r="O24" s="52"/>
+      <c r="P24" s="35"/>
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
       <c r="S24" s="4"/>
@@ -8243,21 +8318,21 @@
     </row>
     <row r="25" spans="1:26" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="44"/>
-      <c r="K25" s="44"/>
-      <c r="L25" s="44"/>
-      <c r="M25" s="44"/>
-      <c r="N25" s="44"/>
-      <c r="O25" s="44"/>
-      <c r="P25" s="45"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="43"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
@@ -9807,6 +9882,11 @@
     <row r="1020" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="L15:L17"/>
+    <mergeCell ref="M15:O17"/>
+    <mergeCell ref="E19:O20"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="C19:D20"/>
     <mergeCell ref="C22:D24"/>
@@ -9823,11 +9903,6 @@
     <mergeCell ref="D15:E17"/>
     <mergeCell ref="G15:G17"/>
     <mergeCell ref="H15:J17"/>
-    <mergeCell ref="L15:L17"/>
-    <mergeCell ref="M15:O17"/>
-    <mergeCell ref="E19:O20"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
   </mergeCells>
   <conditionalFormatting sqref="H10:I11">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">

</xml_diff>